<commit_message>
Aggiunto file per modificare la macro, ogni volta, quindi ora ad ogni ricerca si aggiorna la macro, in modo che riprenda sempre dalla ricerca in cui si è fermato. Inoltre aggiunta funziona per modificare l'excel passandogli cella e testo da inserire. Utile per modificare la macro
</commit_message>
<xml_diff>
--- a/file/macro.xlsx
+++ b/file/macro.xlsx
@@ -1,113 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
-  <si>
-    <t>Numero processo</t>
-  </si>
-  <si>
-    <t>Processi</t>
-  </si>
-  <si>
-    <t>Ricerca</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Carta A4 per stampanti (80 g/m²)</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Carta igienica (3 veli, 50 m)</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Rotoli jumbo e mini-jumbo</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>Asciugamani monouso in rotolo o piegati</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>Fazzoletti per il naso</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>Rotoli industriali grandi</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>Quaderni, block-notes, agende</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>Carta da cucina riutilizzabile</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>Panni per la pulizia in bambù</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>Tovaglioli, tovagliette e scatole in carta di bambù</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>Etichette compostabili e buste per spedizioni</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -125,25 +45,90 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -431,129 +416,186 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="2" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col width="16.71928571428571" bestFit="1" customWidth="1" style="3" min="1" max="1"/>
+    <col width="12.43357142857143" bestFit="1" customWidth="1" style="3" min="2" max="2"/>
+    <col width="12.43357142857143" bestFit="1" customWidth="1" style="3" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>24</v>
+    <row r="1" ht="17.25" customHeight="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>NumeroProcesso</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Processi</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Ricerca</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="17.25" customHeight="1">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>Carta A4 per stampanti (80 g/m²)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="17.25" customHeight="1">
+      <c r="A3" s="3" t="n"/>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>Carta igienica (3 veli, 50 m)</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="17.25" customHeight="1">
+      <c r="A4" s="3" t="n"/>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>Rotoli jumbo e mini-jumbo</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="17.25" customHeight="1">
+      <c r="A5" s="3" t="n"/>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>Asciugamani monouso in rotolo o piegati</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="17.25" customHeight="1">
+      <c r="A6" s="3" t="n"/>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>Fazzoletti per il naso</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="17.25" customHeight="1">
+      <c r="A7" s="3" t="n"/>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>Rotoli industriali grandi</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="17.25" customHeight="1">
+      <c r="A8" s="3" t="n"/>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="C8" s="3" t="inlineStr">
+        <is>
+          <t>Quaderni, block-notes, agende</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="17.25" customHeight="1">
+      <c r="A9" s="3" t="n"/>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>Carta da cucina riutilizzabile</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="17.25" customHeight="1">
+      <c r="A10" s="3" t="n"/>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>Panni per la pulizia in bambù</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="17.25" customHeight="1">
+      <c r="A11" s="3" t="n"/>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>Tovaglioli, tovagliette e scatole in carta di bambù</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="17.25" customHeight="1">
+      <c r="A12" s="3" t="n"/>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>Etichette compostabili e buste per spedizioni</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
aggiunta funzione che mi restituisce il top delle aziende, con quante volte appare, in quale ricerca
</commit_message>
<xml_diff>
--- a/file/macro.xlsx
+++ b/file/macro.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,6 +469,11 @@
           <t>Ricerca</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Nome</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -483,7 +488,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Carta A4 per stampanti 80 g m² all'ingrosso | A4 copy paper supplier bulk office printing paper manufacturer</t>
+          <t>bamboo toilet paper 5 ply 50m bamboo core 100 percent bamboo pulp plastic free FSC Ecolabel OEM</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Carta igienica</t>
         </is>
       </c>
     </row>
@@ -495,7 +505,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Carta igienica 3 veli 50 m ecologica all'ingrosso | toilet paper 3 ply 50m eco-friendly bulk supplier manufacturer</t>
+          <t>bamboo jumbo tissue roll large and mini jumbo 100 percent bamboo pulp plastic free FSC OEM</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Rotolo jumbo</t>
         </is>
       </c>
     </row>
@@ -507,7 +522,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Rotoli jumbo e mini-jumbo carta tissue industriale all'ingrosso | jumbo mini jumbo tissue paper rolls manufacturer supplier</t>
+          <t>bamboo paper hand towels roll or folded 100 percent bamboo pulp plastic free FSC OEM</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Asciugamani carta</t>
         </is>
       </c>
     </row>
@@ -519,7 +539,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Asciugamani monouso in rotolo o piegati per bagno e hotel | disposable hand towels roll folded paper towel bulk supplier</t>
+          <t>A4 copy paper 80gsm 100 percent bamboo pulp plastic free FSC Ecolabel OEM custom logo</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Carta A4</t>
         </is>
       </c>
     </row>
@@ -531,7 +556,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Fazzoletti per il naso morbidi e confezionati all'ingrosso | soft facial tissues pocket pack manufacturer supplier</t>
+          <t>notebooks and bloc-notes bamboo paper pages kraft cover plastic free FSC custom logo</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Quaderni blocchi</t>
         </is>
       </c>
     </row>
@@ -543,7 +573,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Rotoli industriali grandi carta per pulizia officina | large industrial cleaning paper rolls bulk supplier manufacturer</t>
+          <t>facial tissues 100 percent bamboo pulp pocket or box plastic free FSC Ecolabel OEM</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Fazzoletti naso</t>
         </is>
       </c>
     </row>
@@ -555,7 +590,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Quaderni, block-notes e agende personalizzabili all'ingrosso | notebooks journals planners custom logo wholesale manufacturer</t>
+          <t>kraft paper tape water-activated gummed biodegradable plastic free FSC custom print</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Nastro kraft</t>
         </is>
       </c>
     </row>
@@ -567,43 +607,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Carta da cucina riutilizzabile e assorbente ecologica | reusable kitchen paper towels eco-friendly cleaning rolls supplier</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Panni per la pulizia in bambù biodegradabili | bamboo cleaning cloths reusable eco-friendly wipes manufacturer supplier</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Tovaglioli, tovagliette e scatole in carta di bambù compostabili | bamboo napkins placemats packaging eco compostable supplier</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Etichette compostabili e buste per spedizioni ecologiche | compostable shipping labels and packaging mailers manufacturer</t>
+          <t>bamboo kraft recycled paper packaging boxes and mailers plastic free FSC custom branding</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Packaging carta</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
ora mi mette tutte le parole chiave affianco
</commit_message>
<xml_diff>
--- a/file/macro.xlsx
+++ b/file/macro.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr codeName="ThisWorkbook"/>
+  <workbookPr/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+  </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -17,7 +22,7 @@
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
-      <sz val="12"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -45,9 +50,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -194,7 +199,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -229,7 +233,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -264,16 +267,20 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -395,46 +402,7 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
@@ -445,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,16 +439,11 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Nome</t>
+          <t>ParoleChiave</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>1</t>
@@ -493,7 +456,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Carta igienica</t>
+          <t>packaging sostenibile</t>
         </is>
       </c>
     </row>
@@ -510,7 +473,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Rotolo jumbo</t>
+          <t>imballaggio sostenibile</t>
         </is>
       </c>
     </row>
@@ -527,7 +490,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Asciugamani carta</t>
+          <t>packaging ecologico</t>
         </is>
       </c>
     </row>
@@ -544,7 +507,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Carta A4</t>
+          <t>imballaggio ecologico</t>
         </is>
       </c>
     </row>
@@ -561,7 +524,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Quaderni blocchi</t>
+          <t>packaging biodegradabile</t>
         </is>
       </c>
     </row>
@@ -578,7 +541,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Fazzoletti naso</t>
+          <t>packaging compostabile</t>
         </is>
       </c>
     </row>
@@ -595,7 +558,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Nastro kraft</t>
+          <t>packaging riciclabile</t>
         </is>
       </c>
     </row>
@@ -612,7 +575,202 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Packaging carta</t>
+          <t>imballaggio riciclabile</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>carta kraft</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>carta riciclata</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>cellulosa di bambù</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>fibra di bambù</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>materiale riciclato</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>materiale ecologico</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>materiale sostenibile</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>bambù</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>campione gratuito</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>spedizione campioni</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>campione personalizzato</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>packaging personalizzato</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>imballaggio personalizzato</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>scatola ecologica</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>scatola sostenibile</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
tuttoCompreso.py migliorie piu migliori log
</commit_message>
<xml_diff>
--- a/file/macro.xlsx
+++ b/file/macro.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
-  <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
-  </bookViews>
+  <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -22,7 +17,7 @@
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
-      <sz val="11"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -50,9 +45,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -199,6 +194,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -233,6 +229,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -267,20 +264,16 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -402,7 +395,46 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
@@ -413,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,8 +474,18 @@
           <t>ParoleChiave</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Nome</t>
+        </is>
+      </c>
     </row>
     <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>1</t>
@@ -457,6 +499,11 @@
       <c r="D2" t="inlineStr">
         <is>
           <t>packaging sostenibile</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Carta</t>
         </is>
       </c>
     </row>
@@ -476,6 +523,11 @@
           <t>imballaggio sostenibile</t>
         </is>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Bamboo</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="B4" t="inlineStr">
@@ -493,6 +545,11 @@
           <t>packaging ecologico</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Paper</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="B5" t="inlineStr">
@@ -510,6 +567,11 @@
           <t>imballaggio ecologico</t>
         </is>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>A4</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="B6" t="inlineStr">
@@ -527,6 +589,11 @@
           <t>packaging biodegradabile</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>notebooks</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="B7" t="inlineStr">
@@ -541,7 +608,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>packaging compostabile</t>
+          <t>imballaggio biodegradabile</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>facial tissues</t>
         </is>
       </c>
     </row>
@@ -558,7 +630,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>packaging riciclabile</t>
+          <t>packaging compostabile</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Kraft Paper</t>
         </is>
       </c>
     </row>
@@ -575,202 +652,187 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
+          <t>imballaggio compostabile</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Kraft recycled</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>packaging riciclabile</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="D11" t="inlineStr">
+        <is>
           <t>imballaggio riciclabile</t>
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr">
+    <row r="12">
+      <c r="D12" t="inlineStr">
         <is>
           <t>carta kraft</t>
         </is>
       </c>
     </row>
-    <row r="11">
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr">
+    <row r="13">
+      <c r="D13" t="inlineStr">
         <is>
           <t>carta riciclata</t>
         </is>
       </c>
     </row>
-    <row r="12">
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr">
+    <row r="14">
+      <c r="D14" t="inlineStr">
         <is>
           <t>cellulosa di bambù</t>
         </is>
       </c>
     </row>
-    <row r="13">
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr">
+    <row r="15">
+      <c r="D15" t="inlineStr">
         <is>
           <t>fibra di bambù</t>
         </is>
       </c>
     </row>
-    <row r="14">
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr">
+    <row r="16">
+      <c r="D16" t="inlineStr">
         <is>
           <t>materiale riciclato</t>
         </is>
       </c>
     </row>
-    <row r="15">
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr">
+    <row r="17">
+      <c r="D17" t="inlineStr">
         <is>
           <t>materiale ecologico</t>
         </is>
       </c>
     </row>
-    <row r="16">
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr">
+    <row r="18">
+      <c r="D18" t="inlineStr">
         <is>
           <t>materiale sostenibile</t>
         </is>
       </c>
     </row>
-    <row r="17">
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr">
+    <row r="19">
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>bambù naturale</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>cartone riciclato</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>eco friendly</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>prodotto ecologico</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>scatola ecologica</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>scatola sostenibile</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>packaging personalizzato</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>imballaggio personalizzato</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>stampa personalizzata</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>etichetta ecologica</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>busta compostabile</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>sacchetto biodegradabile</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>spedizione campioni</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>bambu</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="D33" t="inlineStr">
         <is>
           <t>bambù</t>
         </is>
       </c>
     </row>
-    <row r="18">
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>campione gratuito</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>spedizione campioni</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>campione personalizzato</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>packaging personalizzato</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>imballaggio personalizzato</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>scatola ecologica</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>scatola sostenibile</t>
+    <row r="34">
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>kraft</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Aggiustato topAziende e inserita funzione che logga dentro la cartella dei log
</commit_message>
<xml_diff>
--- a/file/macro.xlsx
+++ b/file/macro.xlsx
@@ -483,17 +483,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>bamboo toilet paper 5 ply 50m bamboo core 100 percent bamboo pulp plastic free FSC Ecolabel OEM</t>
+          <t>test</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -515,7 +515,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>bamboo jumbo tissue roll large and mini jumbo 100 percent bamboo pulp plastic free FSC OEM</t>
+          <t>test2</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -525,29 +525,14 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>pop</t>
+          <t>ee</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>ciao</t>
-        </is>
-      </c>
       <c r="D4" t="inlineStr">
         <is>
           <t>packaging ecologico</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>ciao</t>
         </is>
       </c>
     </row>

</xml_diff>